<commit_message>
Totals added to export.
</commit_message>
<xml_diff>
--- a/code/Client Records/BillingWinForms/bin/Release/ClientRecordsTEMPLATE.xlsx
+++ b/code/Client Records/BillingWinForms/bin/Release/ClientRecordsTEMPLATE.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -99,20 +99,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -330,62 +324,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,7 +688,7 @@
   <dimension ref="B1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,93 +706,93 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="21" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="22" t="s">
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="23"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="20"/>
     </row>
     <row r="3" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="18"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="24" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26" t="s">
+      <c r="F3" s="31"/>
+      <c r="G3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="32"/>
+      <c r="I3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26" t="s">
+      <c r="J3" s="31"/>
+      <c r="K3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="24" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="25"/>
-      <c r="O3" s="30" t="s">
+      <c r="N3" s="31"/>
+      <c r="O3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="27" t="s">
+      <c r="P3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="32" t="s">
+      <c r="R3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="27" t="s">
+      <c r="S3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="30" t="s">
+      <c r="T3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="U3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="28" t="s">
+      <c r="V3" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="14" t="s">
         <v>10</v>
       </c>
@@ -829,14 +823,14 @@
       <c r="N4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="31"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="29"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="22"/>
     </row>
     <row r="5" spans="2:22" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
@@ -924,28 +918,94 @@
         <v>15</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="4"/>
+      <c r="D8" s="4">
+        <f>SUM(D5:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f>(SUM(E5:E7))</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" ref="F8:V8" si="0">(SUM(F5:F7))</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:N2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -956,15 +1016,6 @@
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:N2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mouse Cursos changed while processing. DateTime comparison bug at table before excel export fixed. (hours, mins, seconds are set to 0) On main window dateFrom is Jan1 current year, dayUntil is current day. Totals are updated correctly on excel table. Count calculations at excel table optimized a bit, but can do better. (with Maps)
</commit_message>
<xml_diff>
--- a/code/Client Records/BillingWinForms/bin/Release/ClientRecordsTEMPLATE.xlsx
+++ b/code/Client Records/BillingWinForms/bin/Release/ClientRecordsTEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Examinari in functie de localizare</t>
   </si>
@@ -94,6 +94,15 @@
       </rPr>
       <t xml:space="preserve"> 40ani</t>
     </r>
+  </si>
+  <si>
+    <t>0df</t>
+  </si>
+  <si>
+    <t>0gg</t>
+  </si>
+  <si>
+    <t>1gggg</t>
   </si>
 </sst>
 </file>
@@ -333,16 +342,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -359,27 +389,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,93 +715,93 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="18" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="19" t="s">
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="20"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="23"/>
     </row>
     <row r="3" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="27"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="30" t="s">
+      <c r="H3" s="26"/>
+      <c r="I3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="25"/>
+      <c r="K3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="30" t="s">
+      <c r="L3" s="26"/>
+      <c r="M3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="31"/>
-      <c r="O3" s="23" t="s">
+      <c r="N3" s="25"/>
+      <c r="O3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="23" t="s">
+      <c r="Q3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="25" t="s">
+      <c r="R3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="S3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="23" t="s">
+      <c r="T3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="U3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="27"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="14" t="s">
         <v>10</v>
       </c>
@@ -823,14 +832,14 @@
       <c r="N4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="24"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="22"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="29"/>
     </row>
     <row r="5" spans="2:22" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
@@ -839,17 +848,39 @@
       <c r="C5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="8"/>
+      <c r="D5" s="8">
+        <v>650</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <v>9</v>
+      </c>
+      <c r="J5" s="8">
+        <v>13</v>
+      </c>
+      <c r="K5" s="7">
+        <v>119</v>
+      </c>
+      <c r="L5" s="8">
+        <v>219</v>
+      </c>
+      <c r="M5" s="5">
+        <v>114</v>
+      </c>
+      <c r="N5" s="8">
+        <v>175</v>
+      </c>
       <c r="O5" s="8"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="8"/>
@@ -919,51 +950,40 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4">
-        <f>SUM(D5:D7)</f>
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="E8" s="1">
-        <f>(SUM(E5:E7))</f>
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:V8" si="0">(SUM(F5:F7))</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F8:V8" si="0">(SUM(O5:O7))</f>
         <v>0</v>
       </c>
       <c r="P8" s="1">
@@ -997,15 +1017,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:N2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -1016,6 +1027,15 @@
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:N2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>